<commit_message>
Deploy: include XLSX + generated JSON; ensure prebuild runs
</commit_message>
<xml_diff>
--- a/data/input/q2-2025.xlsx
+++ b/data/input/q2-2025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ciwhisky-my.sharepoint.com/personal/campbell_csca_co_uk/Documents/_CSCA/BlueNord/bluenord-clean/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/campbellshirlaw/DevProjects/bluenord-green/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{F6E9F7B3-E725-BD44-AD9F-6F936B62D3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{535E173D-C13D-1B4A-A1E8-2919CEBDE3E1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2448D58-F443-044E-B493-D18656B598DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16760" activeTab="1" xr2:uid="{41D02D6D-6253-A846-8E6A-EE5BA2F37BF2}"/>
+    <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16760" activeTab="8" xr2:uid="{41D02D6D-6253-A846-8E6A-EE5BA2F37BF2}"/>
   </bookViews>
   <sheets>
     <sheet name="kpis" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t>text</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>50–70% of operating cash flow</t>
+  </si>
+  <si>
+    <t>Wins</t>
+  </si>
+  <si>
+    <t>games</t>
+  </si>
+  <si>
+    <t>football</t>
   </si>
 </sst>
 </file>
@@ -522,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2EA804-DB2C-A244-9769-9D7B5869862C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,6 +551,20 @@
       </c>
       <c r="D1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F76F5680-097B-A24F-9D12-6E60C7E3181B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -698,10 +721,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89021A8D-B9A8-C347-81B4-5D68A712D360}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,6 +740,50 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45748</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45778</v>
+      </c>
+      <c r="B3">
+        <v>110</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45809</v>
+      </c>
+      <c r="B4">
+        <v>120</v>
+      </c>
+      <c r="C4">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45839</v>
+      </c>
+      <c r="B5">
+        <v>140</v>
+      </c>
+      <c r="C5">
+        <v>1.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -725,10 +792,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490C1938-7F4E-C44E-90CA-E19A2FBAD111}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -742,6 +809,50 @@
       </c>
       <c r="C1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>45748</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45778</v>
+      </c>
+      <c r="B3">
+        <v>244</v>
+      </c>
+      <c r="C3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45809</v>
+      </c>
+      <c r="B4">
+        <v>299</v>
+      </c>
+      <c r="C4">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45839</v>
+      </c>
+      <c r="B5">
+        <v>140</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45C11D8-3D9B-E645-9797-DE0D30EDBD17}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>